<commit_message>
MOS i PANAS i EPT añadidos. Falta arreglar nombres variables PANAS.
</commit_message>
<xml_diff>
--- a/TFG/res/pacientData/100101/Resultats_REM-G100101.xlsx
+++ b/TFG/res/pacientData/100101/Resultats_REM-G100101.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="573">
   <si>
     <t>ID</t>
   </si>
@@ -743,6 +743,18 @@
     <t>FV - Animals_T1</t>
   </si>
   <si>
+    <t>Fluencia verbal NSSA - P_T1</t>
+  </si>
+  <si>
+    <t>FV NSSA - M_T1</t>
+  </si>
+  <si>
+    <t>FV NSSA - R_T1</t>
+  </si>
+  <si>
+    <t>FV NSSA - Animals_T1</t>
+  </si>
+  <si>
     <t>EPT_T1</t>
   </si>
   <si>
@@ -782,6 +794,39 @@
     <t>IMAGE_T1</t>
   </si>
   <si>
+    <t>PANAS_afect-positivo_T1</t>
+  </si>
+  <si>
+    <t>PANAS_afect-negativo_T1</t>
+  </si>
+  <si>
+    <t>PANAS_TOTAL_T1</t>
+  </si>
+  <si>
+    <t>MOS_Amigos_T1</t>
+  </si>
+  <si>
+    <t>MOS_Familia_T1</t>
+  </si>
+  <si>
+    <t>MOS_ApoyoEmocional_T1</t>
+  </si>
+  <si>
+    <t>MOS_AyudaMaterial_T1</t>
+  </si>
+  <si>
+    <t>MOS_SocialOcio_T1</t>
+  </si>
+  <si>
+    <t>MOS_ApoyoAfectivo_T1</t>
+  </si>
+  <si>
+    <t>MOS_TOTAL_T1</t>
+  </si>
+  <si>
+    <t>EPTTotalCuidador_T1</t>
+  </si>
+  <si>
     <t>FAQ_T1</t>
   </si>
   <si>
@@ -1112,6 +1157,18 @@
     <t>FV - Animals_T2</t>
   </si>
   <si>
+    <t>Fluencia verbal NSSA - P_T2</t>
+  </si>
+  <si>
+    <t>FV NSSA - M_T2</t>
+  </si>
+  <si>
+    <t>FV NSSA - R_T2</t>
+  </si>
+  <si>
+    <t>FV NSSA - Animals_T2</t>
+  </si>
+  <si>
     <t>EPT_T2</t>
   </si>
   <si>
@@ -1151,6 +1208,39 @@
     <t>IMAGE_T2</t>
   </si>
   <si>
+    <t>PANAS_afect-positivo_T2</t>
+  </si>
+  <si>
+    <t>PANAS_afect-negativo_T2</t>
+  </si>
+  <si>
+    <t>PANAS_TOTAL_T2</t>
+  </si>
+  <si>
+    <t>MOS_Amigos_T2</t>
+  </si>
+  <si>
+    <t>MOS_Familia_T2</t>
+  </si>
+  <si>
+    <t>MOS_ApoyoEmocional_T2</t>
+  </si>
+  <si>
+    <t>MOS_AyudaMaterial_T2</t>
+  </si>
+  <si>
+    <t>MOS_SocialOcio_T2</t>
+  </si>
+  <si>
+    <t>MOS_ApoyoAfectivo_T2</t>
+  </si>
+  <si>
+    <t>MOS_TOTAL_T2</t>
+  </si>
+  <si>
+    <t>EPTTotalCuidador_T2</t>
+  </si>
+  <si>
     <t>FAQ_T2</t>
   </si>
   <si>
@@ -1481,6 +1571,18 @@
     <t>FV - Animals_T3</t>
   </si>
   <si>
+    <t>Fluencia verbal NSSA - P_T3</t>
+  </si>
+  <si>
+    <t>FV NSSA - M_T3</t>
+  </si>
+  <si>
+    <t>FV NSSA - R_T3</t>
+  </si>
+  <si>
+    <t>FV NSSA - Animals_T3</t>
+  </si>
+  <si>
     <t>EPT_T3</t>
   </si>
   <si>
@@ -1520,6 +1622,39 @@
     <t>IMAGE_T3</t>
   </si>
   <si>
+    <t>PANAS_afect-positivo_T3</t>
+  </si>
+  <si>
+    <t>PANAS_afect-negativo_T3</t>
+  </si>
+  <si>
+    <t>PANAS_TOTAL_T3</t>
+  </si>
+  <si>
+    <t>MOS_Amigos_T3</t>
+  </si>
+  <si>
+    <t>MOS_Familia_T3</t>
+  </si>
+  <si>
+    <t>MOS_ApoyoEmocional_T3</t>
+  </si>
+  <si>
+    <t>MOS_AyudaMaterial_T3</t>
+  </si>
+  <si>
+    <t>MOS_SocialOcio_T3</t>
+  </si>
+  <si>
+    <t>MOS_ApoyoAfectivo_T3</t>
+  </si>
+  <si>
+    <t>MOS_TOTAL_T3</t>
+  </si>
+  <si>
+    <t>EPTTotalCuidador_T3</t>
+  </si>
+  <si>
     <t>FAQ_T3</t>
   </si>
   <si>
@@ -1581,6 +1716,21 @@
   </si>
   <si>
     <t>Ara no, anteriorment sí (fa més de 12 mesos que no en fa)</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>15</t>
   </si>
 </sst>
 </file>
@@ -2593,19 +2743,19 @@
         <v>242</v>
       </c>
       <c r="LI1" t="s">
-        <v>137</v>
+        <v>243</v>
       </c>
       <c r="LJ1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="LK1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="LL1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="LM1" t="s">
-        <v>246</v>
+        <v>137</v>
       </c>
       <c r="LN1" t="s">
         <v>247</v>
@@ -2635,79 +2785,79 @@
         <v>255</v>
       </c>
       <c r="LW1" t="s">
-        <v>137</v>
+        <v>256</v>
       </c>
       <c r="LX1" t="s">
+        <v>257</v>
+      </c>
+      <c r="LY1" t="s">
+        <v>258</v>
+      </c>
+      <c r="LZ1" t="s">
+        <v>259</v>
+      </c>
+      <c r="MA1" t="s">
+        <v>260</v>
+      </c>
+      <c r="MB1" t="s">
+        <v>261</v>
+      </c>
+      <c r="MC1" t="s">
+        <v>262</v>
+      </c>
+      <c r="MD1" t="s">
+        <v>263</v>
+      </c>
+      <c r="ME1" t="s">
+        <v>264</v>
+      </c>
+      <c r="MF1" t="s">
+        <v>265</v>
+      </c>
+      <c r="MG1" t="s">
+        <v>266</v>
+      </c>
+      <c r="MH1" t="s">
+        <v>267</v>
+      </c>
+      <c r="MI1" t="s">
+        <v>268</v>
+      </c>
+      <c r="MJ1" t="s">
+        <v>269</v>
+      </c>
+      <c r="MK1" t="s">
+        <v>137</v>
+      </c>
+      <c r="ML1" t="s">
+        <v>270</v>
+      </c>
+      <c r="MM1" t="s">
+        <v>271</v>
+      </c>
+      <c r="MN1" t="s">
+        <v>272</v>
+      </c>
+      <c r="MO1" t="s">
+        <v>253</v>
+      </c>
+      <c r="MP1" t="s">
+        <v>254</v>
+      </c>
+      <c r="MQ1" t="s">
+        <v>273</v>
+      </c>
+      <c r="MR1" t="s">
+        <v>274</v>
+      </c>
+      <c r="MS1" t="s">
         <v>256</v>
       </c>
-      <c r="LY1" t="s">
-        <v>257</v>
-      </c>
-      <c r="LZ1" t="s">
-        <v>249</v>
-      </c>
-      <c r="MA1" t="s">
-        <v>250</v>
-      </c>
-      <c r="MB1" t="s">
-        <v>258</v>
-      </c>
-      <c r="MC1" t="s">
-        <v>259</v>
-      </c>
-      <c r="MD1" t="s">
-        <v>252</v>
-      </c>
-      <c r="ME1" t="s">
-        <v>260</v>
-      </c>
-      <c r="MF1" t="s">
-        <v>137</v>
-      </c>
-      <c r="MG1" t="s">
-        <v>261</v>
-      </c>
-      <c r="MH1" t="s">
-        <v>262</v>
-      </c>
-      <c r="MI1" t="s">
-        <v>263</v>
-      </c>
-      <c r="MJ1" t="s">
-        <v>264</v>
-      </c>
-      <c r="MK1" t="s">
-        <v>265</v>
-      </c>
-      <c r="ML1" t="s">
-        <v>266</v>
-      </c>
-      <c r="MM1" t="s">
-        <v>267</v>
-      </c>
-      <c r="MN1" t="s">
-        <v>268</v>
-      </c>
-      <c r="MO1" t="s">
-        <v>269</v>
-      </c>
-      <c r="MP1" t="s">
-        <v>270</v>
-      </c>
-      <c r="MQ1" t="s">
-        <v>271</v>
-      </c>
-      <c r="MR1" t="s">
-        <v>272</v>
-      </c>
-      <c r="MS1" t="s">
-        <v>273</v>
-      </c>
       <c r="MT1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="MU1" t="s">
-        <v>275</v>
+        <v>137</v>
       </c>
       <c r="MV1" t="s">
         <v>276</v>
@@ -2980,166 +3130,166 @@
         <v>365</v>
       </c>
       <c r="QH1" t="s">
-        <v>137</v>
+        <v>366</v>
       </c>
       <c r="QI1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="QJ1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="QK1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="QL1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="QM1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="QN1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="QO1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="QP1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="QQ1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="QR1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="QS1" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="QT1" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="QU1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="QV1" t="s">
-        <v>137</v>
+        <v>380</v>
       </c>
       <c r="QW1" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="QX1" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="QY1" t="s">
-        <v>372</v>
+        <v>383</v>
       </c>
       <c r="QZ1" t="s">
-        <v>373</v>
+        <v>384</v>
       </c>
       <c r="RA1" t="s">
-        <v>381</v>
+        <v>137</v>
       </c>
       <c r="RB1" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="RC1" t="s">
-        <v>375</v>
+        <v>386</v>
       </c>
       <c r="RD1" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="RE1" t="s">
-        <v>137</v>
+        <v>388</v>
       </c>
       <c r="RF1" t="s">
-        <v>384</v>
+        <v>389</v>
       </c>
       <c r="RG1" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="RH1" t="s">
-        <v>386</v>
+        <v>391</v>
       </c>
       <c r="RI1" t="s">
-        <v>387</v>
+        <v>392</v>
       </c>
       <c r="RJ1" t="s">
-        <v>388</v>
+        <v>393</v>
       </c>
       <c r="RK1" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="RL1" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="RM1" t="s">
+        <v>396</v>
+      </c>
+      <c r="RN1" t="s">
+        <v>397</v>
+      </c>
+      <c r="RO1" t="s">
+        <v>398</v>
+      </c>
+      <c r="RP1" t="s">
+        <v>399</v>
+      </c>
+      <c r="RQ1" t="s">
+        <v>400</v>
+      </c>
+      <c r="RR1" t="s">
+        <v>401</v>
+      </c>
+      <c r="RS1" t="s">
+        <v>402</v>
+      </c>
+      <c r="RT1" t="s">
+        <v>403</v>
+      </c>
+      <c r="RU1" t="s">
+        <v>404</v>
+      </c>
+      <c r="RV1" t="s">
+        <v>405</v>
+      </c>
+      <c r="RW1" t="s">
+        <v>406</v>
+      </c>
+      <c r="RX1" t="s">
+        <v>407</v>
+      </c>
+      <c r="RY1" t="s">
+        <v>137</v>
+      </c>
+      <c r="RZ1" t="s">
+        <v>408</v>
+      </c>
+      <c r="SA1" t="s">
+        <v>409</v>
+      </c>
+      <c r="SB1" t="s">
+        <v>410</v>
+      </c>
+      <c r="SC1" t="s">
         <v>391</v>
       </c>
-      <c r="RN1" t="s">
+      <c r="SD1" t="s">
         <v>392</v>
       </c>
-      <c r="RO1" t="s">
-        <v>393</v>
-      </c>
-      <c r="RP1" t="s">
+      <c r="SE1" t="s">
+        <v>411</v>
+      </c>
+      <c r="SF1" t="s">
+        <v>412</v>
+      </c>
+      <c r="SG1" t="s">
         <v>394</v>
       </c>
-      <c r="RQ1" t="s">
-        <v>395</v>
-      </c>
-      <c r="RR1" t="s">
-        <v>396</v>
-      </c>
-      <c r="RS1" t="s">
-        <v>397</v>
-      </c>
-      <c r="RT1" t="s">
-        <v>398</v>
-      </c>
-      <c r="RU1" t="s">
-        <v>399</v>
-      </c>
-      <c r="RV1" t="s">
-        <v>400</v>
-      </c>
-      <c r="RW1" t="s">
-        <v>401</v>
-      </c>
-      <c r="RX1" t="s">
-        <v>402</v>
-      </c>
-      <c r="RY1" t="s">
-        <v>403</v>
-      </c>
-      <c r="RZ1" t="s">
-        <v>404</v>
-      </c>
-      <c r="SA1" t="s">
-        <v>405</v>
-      </c>
-      <c r="SB1" t="s">
-        <v>406</v>
-      </c>
-      <c r="SC1" t="s">
-        <v>407</v>
-      </c>
-      <c r="SD1" t="s">
-        <v>408</v>
-      </c>
-      <c r="SE1" t="s">
-        <v>409</v>
-      </c>
-      <c r="SF1" t="s">
-        <v>410</v>
-      </c>
-      <c r="SG1" t="s">
-        <v>411</v>
-      </c>
       <c r="SH1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="SI1" t="s">
-        <v>413</v>
+        <v>137</v>
       </c>
       <c r="SJ1" t="s">
         <v>414</v>
@@ -3367,144 +3517,1377 @@
         <v>488</v>
       </c>
       <c r="VG1" t="s">
-        <v>137</v>
+        <v>489</v>
       </c>
       <c r="VH1" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="VI1" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="VJ1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="VK1" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="VL1" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="VM1" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="VN1" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="VO1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="VP1" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="VQ1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="VR1" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="VS1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="VT1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="VU1" t="s">
-        <v>137</v>
+        <v>503</v>
       </c>
       <c r="VV1" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="VW1" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="VX1" t="s">
-        <v>495</v>
+        <v>506</v>
       </c>
       <c r="VY1" t="s">
-        <v>496</v>
+        <v>507</v>
       </c>
       <c r="VZ1" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="WA1" t="s">
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="WB1" t="s">
-        <v>498</v>
+        <v>510</v>
       </c>
       <c r="WC1" t="s">
-        <v>506</v>
+        <v>511</v>
+      </c>
+      <c r="WD1" t="s">
+        <v>512</v>
+      </c>
+      <c r="WE1" t="s">
+        <v>513</v>
+      </c>
+      <c r="WF1" t="s">
+        <v>514</v>
+      </c>
+      <c r="WG1" t="s">
+        <v>515</v>
+      </c>
+      <c r="WH1" t="s">
+        <v>516</v>
+      </c>
+      <c r="WI1" t="s">
+        <v>517</v>
+      </c>
+      <c r="WJ1" t="s">
+        <v>518</v>
+      </c>
+      <c r="WK1" t="s">
+        <v>519</v>
+      </c>
+      <c r="WL1" t="s">
+        <v>520</v>
+      </c>
+      <c r="WM1" t="s">
+        <v>521</v>
+      </c>
+      <c r="WN1" t="s">
+        <v>522</v>
+      </c>
+      <c r="WO1" t="s">
+        <v>137</v>
+      </c>
+      <c r="WP1" t="s">
+        <v>523</v>
+      </c>
+      <c r="WQ1" t="s">
+        <v>524</v>
+      </c>
+      <c r="WR1" t="s">
+        <v>525</v>
+      </c>
+      <c r="WS1" t="s">
+        <v>526</v>
+      </c>
+      <c r="WT1" t="s">
+        <v>527</v>
+      </c>
+      <c r="WU1" t="s">
+        <v>528</v>
+      </c>
+      <c r="WV1" t="s">
+        <v>529</v>
+      </c>
+      <c r="WW1" t="s">
+        <v>530</v>
+      </c>
+      <c r="WX1" t="s">
+        <v>531</v>
+      </c>
+      <c r="WY1" t="s">
+        <v>532</v>
+      </c>
+      <c r="WZ1" t="s">
+        <v>533</v>
+      </c>
+      <c r="XA1" t="s">
+        <v>534</v>
+      </c>
+      <c r="XB1" t="s">
+        <v>535</v>
+      </c>
+      <c r="XC1" t="s">
+        <v>536</v>
+      </c>
+      <c r="XD1" t="s">
+        <v>537</v>
+      </c>
+      <c r="XE1" t="s">
+        <v>538</v>
+      </c>
+      <c r="XF1" t="s">
+        <v>539</v>
+      </c>
+      <c r="XG1" t="s">
+        <v>540</v>
+      </c>
+      <c r="XH1" t="s">
+        <v>541</v>
+      </c>
+      <c r="XI1" t="s">
+        <v>542</v>
+      </c>
+      <c r="XJ1" t="s">
+        <v>543</v>
+      </c>
+      <c r="XK1" t="s">
+        <v>544</v>
+      </c>
+      <c r="XL1" t="s">
+        <v>545</v>
+      </c>
+      <c r="XM1" t="s">
+        <v>137</v>
+      </c>
+      <c r="XN1" t="s">
+        <v>546</v>
+      </c>
+      <c r="XO1" t="s">
+        <v>547</v>
+      </c>
+      <c r="XP1" t="s">
+        <v>548</v>
+      </c>
+      <c r="XQ1" t="s">
+        <v>529</v>
+      </c>
+      <c r="XR1" t="s">
+        <v>530</v>
+      </c>
+      <c r="XS1" t="s">
+        <v>549</v>
+      </c>
+      <c r="XT1" t="s">
+        <v>550</v>
+      </c>
+      <c r="XU1" t="s">
+        <v>532</v>
+      </c>
+      <c r="XV1" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>507</v>
+        <v>552</v>
       </c>
       <c r="B2" t="s">
-        <v>508</v>
+        <v>553</v>
       </c>
       <c r="C2" t="s">
-        <v>509</v>
+        <v>554</v>
       </c>
       <c r="D2" t="s">
-        <v>510</v>
+        <v>555</v>
       </c>
       <c r="E2" t="s">
-        <v>511</v>
+        <v>556</v>
       </c>
       <c r="F2" t="s">
-        <v>512</v>
+        <v>557</v>
       </c>
       <c r="G2" t="s">
-        <v>513</v>
+        <v>558</v>
       </c>
       <c r="H2" t="s">
-        <v>514</v>
+        <v>559</v>
       </c>
       <c r="I2" t="s">
-        <v>515</v>
+        <v>560</v>
       </c>
       <c r="J2" t="s">
-        <v>516</v>
+        <v>561</v>
       </c>
       <c r="K2" t="s">
-        <v>517</v>
+        <v>562</v>
       </c>
       <c r="L2" t="s">
-        <v>518</v>
+        <v>563</v>
       </c>
       <c r="M2" t="s">
-        <v>519</v>
+        <v>564</v>
       </c>
       <c r="N2" t="s">
-        <v>520</v>
+        <v>565</v>
       </c>
       <c r="O2" t="s">
-        <v>520</v>
+        <v>565</v>
       </c>
       <c r="P2" t="s">
-        <v>520</v>
+        <v>565</v>
       </c>
       <c r="Q2" t="s">
         <v>137</v>
       </c>
       <c r="R2" t="s">
-        <v>520</v>
+        <v>565</v>
       </c>
       <c r="S2" t="s">
-        <v>521</v>
+        <v>566</v>
       </c>
       <c r="T2" t="s">
-        <v>520</v>
+        <v>565</v>
       </c>
       <c r="U2" t="s">
-        <v>520</v>
+        <v>565</v>
       </c>
       <c r="V2" t="s">
-        <v>520</v>
+        <v>565</v>
       </c>
       <c r="W2" t="s">
-        <v>522</v>
+        <v>567</v>
+      </c>
+      <c r="X2" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DK2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DS2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DU2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DW2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EA2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EC2" t="s">
+        <v>137</v>
+      </c>
+      <c r="ED2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EE2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EK2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="ER2" t="s">
+        <v>137</v>
+      </c>
+      <c r="ES2" t="s">
+        <v>137</v>
+      </c>
+      <c r="ET2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EU2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EW2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FA2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FC2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FD2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FE2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FK2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FS2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FU2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FW2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GA2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GC2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GD2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GE2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GK2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GS2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GU2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GW2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HA2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HC2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HD2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HE2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HK2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HS2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HU2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HW2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="IA2" t="s">
+        <v>137</v>
+      </c>
+      <c r="IB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="IC2" t="s">
+        <v>137</v>
+      </c>
+      <c r="ID2" t="s">
+        <v>137</v>
+      </c>
+      <c r="IE2" t="s">
+        <v>137</v>
+      </c>
+      <c r="IF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="IG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="IH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="II2" t="s">
+        <v>137</v>
+      </c>
+      <c r="IJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="IK2" t="s">
+        <v>137</v>
+      </c>
+      <c r="IL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="IM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="IN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="IO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="IP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="IQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="IR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="IS2" t="s">
+        <v>137</v>
+      </c>
+      <c r="IT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="IU2" t="s">
+        <v>137</v>
+      </c>
+      <c r="IV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="IW2" t="s">
+        <v>137</v>
+      </c>
+      <c r="IX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="IY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="IZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JA2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JC2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JD2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JE2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JK2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JR2" t="s">
+        <v>568</v>
+      </c>
+      <c r="JS2" t="s">
+        <v>563</v>
+      </c>
+      <c r="JT2" t="s">
+        <v>569</v>
+      </c>
+      <c r="JU2" t="s">
+        <v>569</v>
+      </c>
+      <c r="JV2" t="s">
+        <v>569</v>
+      </c>
+      <c r="JW2" t="s">
+        <v>569</v>
+      </c>
+      <c r="JX2" t="s">
+        <v>569</v>
+      </c>
+      <c r="JY2" t="s">
+        <v>569</v>
+      </c>
+      <c r="JZ2" t="s">
+        <v>569</v>
+      </c>
+      <c r="KA2" t="s">
+        <v>569</v>
+      </c>
+      <c r="KB2" t="s">
+        <v>569</v>
+      </c>
+      <c r="KC2" t="s">
+        <v>569</v>
+      </c>
+      <c r="KD2" t="s">
+        <v>569</v>
+      </c>
+      <c r="KE2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KK2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KP2" t="s">
+        <v>570</v>
+      </c>
+      <c r="KQ2" t="s">
+        <v>569</v>
+      </c>
+      <c r="KR2" t="s">
+        <v>569</v>
+      </c>
+      <c r="KS2" t="s">
+        <v>571</v>
+      </c>
+      <c r="KT2" t="s">
+        <v>571</v>
+      </c>
+      <c r="KU2" t="s">
+        <v>569</v>
+      </c>
+      <c r="KV2" t="s">
+        <v>569</v>
+      </c>
+      <c r="KW2" t="s">
+        <v>569</v>
+      </c>
+      <c r="KX2" t="s">
+        <v>569</v>
+      </c>
+      <c r="KY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LA2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LC2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LD2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LE2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LK2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LS2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LU2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LW2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MA2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MC2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MD2" t="s">
+        <v>137</v>
+      </c>
+      <c r="ME2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MK2" t="s">
+        <v>137</v>
+      </c>
+      <c r="ML2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MS2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MU2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MW2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="NA2" t="s">
+        <v>137</v>
+      </c>
+      <c r="NB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="NC2" t="s">
+        <v>137</v>
+      </c>
+      <c r="ND2" t="s">
+        <v>137</v>
+      </c>
+      <c r="NE2" t="s">
+        <v>137</v>
+      </c>
+      <c r="NF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="NG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="NH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="NI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="NJ2" t="s">
+        <v>569</v>
+      </c>
+      <c r="NK2" t="s">
+        <v>563</v>
+      </c>
+      <c r="NL2" t="s">
+        <v>569</v>
+      </c>
+      <c r="NM2" t="s">
+        <v>569</v>
+      </c>
+      <c r="NN2" t="s">
+        <v>569</v>
+      </c>
+      <c r="NO2" t="s">
+        <v>569</v>
+      </c>
+      <c r="NP2" t="s">
+        <v>569</v>
+      </c>
+      <c r="NQ2" t="s">
+        <v>569</v>
+      </c>
+      <c r="NR2" t="s">
+        <v>569</v>
+      </c>
+      <c r="NS2" t="s">
+        <v>569</v>
+      </c>
+      <c r="NT2" t="s">
+        <v>569</v>
+      </c>
+      <c r="NU2" t="s">
+        <v>569</v>
+      </c>
+      <c r="NV2" t="s">
+        <v>569</v>
+      </c>
+      <c r="NW2" t="s">
+        <v>569</v>
+      </c>
+      <c r="NX2" t="s">
+        <v>572</v>
+      </c>
+      <c r="NY2" t="s">
+        <v>572</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arreglados nombres variabes PANAS
</commit_message>
<xml_diff>
--- a/TFG/res/pacientData/100101/Resultats_REM-G100101.xlsx
+++ b/TFG/res/pacientData/100101/Resultats_REM-G100101.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="572">
   <si>
     <t>ID</t>
   </si>
@@ -1716,9 +1716,6 @@
   </si>
   <si>
     <t>Ara no, anteriorment sí (fa més de 12 mesos que no en fa)</t>
-  </si>
-  <si>
-    <t>7</t>
   </si>
   <si>
     <t>0</t>
@@ -4554,103 +4551,103 @@
         <v>137</v>
       </c>
       <c r="JR2" t="s">
-        <v>568</v>
+        <v>558</v>
       </c>
       <c r="JS2" t="s">
         <v>563</v>
       </c>
       <c r="JT2" t="s">
+        <v>568</v>
+      </c>
+      <c r="JU2" t="s">
+        <v>568</v>
+      </c>
+      <c r="JV2" t="s">
+        <v>568</v>
+      </c>
+      <c r="JW2" t="s">
+        <v>568</v>
+      </c>
+      <c r="JX2" t="s">
+        <v>568</v>
+      </c>
+      <c r="JY2" t="s">
+        <v>568</v>
+      </c>
+      <c r="JZ2" t="s">
+        <v>568</v>
+      </c>
+      <c r="KA2" t="s">
+        <v>568</v>
+      </c>
+      <c r="KB2" t="s">
+        <v>568</v>
+      </c>
+      <c r="KC2" t="s">
+        <v>568</v>
+      </c>
+      <c r="KD2" t="s">
+        <v>568</v>
+      </c>
+      <c r="KE2" t="s">
+        <v>568</v>
+      </c>
+      <c r="KF2" t="s">
+        <v>568</v>
+      </c>
+      <c r="KG2" t="s">
+        <v>568</v>
+      </c>
+      <c r="KH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KJ2" t="s">
+        <v>568</v>
+      </c>
+      <c r="KK2" t="s">
+        <v>568</v>
+      </c>
+      <c r="KL2" t="s">
+        <v>568</v>
+      </c>
+      <c r="KM2" t="s">
+        <v>568</v>
+      </c>
+      <c r="KN2" t="s">
+        <v>568</v>
+      </c>
+      <c r="KO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KP2" t="s">
         <v>569</v>
       </c>
-      <c r="JU2" t="s">
-        <v>569</v>
-      </c>
-      <c r="JV2" t="s">
-        <v>569</v>
-      </c>
-      <c r="JW2" t="s">
-        <v>569</v>
-      </c>
-      <c r="JX2" t="s">
-        <v>569</v>
-      </c>
-      <c r="JY2" t="s">
-        <v>569</v>
-      </c>
-      <c r="JZ2" t="s">
-        <v>569</v>
-      </c>
-      <c r="KA2" t="s">
-        <v>569</v>
-      </c>
-      <c r="KB2" t="s">
-        <v>569</v>
-      </c>
-      <c r="KC2" t="s">
-        <v>569</v>
-      </c>
-      <c r="KD2" t="s">
-        <v>569</v>
-      </c>
-      <c r="KE2" t="s">
-        <v>137</v>
-      </c>
-      <c r="KF2" t="s">
-        <v>137</v>
-      </c>
-      <c r="KG2" t="s">
-        <v>137</v>
-      </c>
-      <c r="KH2" t="s">
-        <v>137</v>
-      </c>
-      <c r="KI2" t="s">
-        <v>137</v>
-      </c>
-      <c r="KJ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="KK2" t="s">
-        <v>137</v>
-      </c>
-      <c r="KL2" t="s">
-        <v>137</v>
-      </c>
-      <c r="KM2" t="s">
-        <v>137</v>
-      </c>
-      <c r="KN2" t="s">
-        <v>137</v>
-      </c>
-      <c r="KO2" t="s">
-        <v>137</v>
-      </c>
-      <c r="KP2" t="s">
+      <c r="KQ2" t="s">
+        <v>568</v>
+      </c>
+      <c r="KR2" t="s">
+        <v>568</v>
+      </c>
+      <c r="KS2" t="s">
         <v>570</v>
       </c>
-      <c r="KQ2" t="s">
-        <v>569</v>
-      </c>
-      <c r="KR2" t="s">
-        <v>569</v>
-      </c>
-      <c r="KS2" t="s">
-        <v>571</v>
-      </c>
       <c r="KT2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="KU2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="KV2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="KW2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="KX2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="KY2" t="s">
         <v>137</v>
@@ -4842,52 +4839,52 @@
         <v>137</v>
       </c>
       <c r="NJ2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="NK2" t="s">
         <v>563</v>
       </c>
       <c r="NL2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="NM2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="NN2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="NO2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="NP2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="NQ2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="NR2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="NS2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="NT2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="NU2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="NV2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="NW2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="NX2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="NY2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
   </sheetData>

</xml_diff>